<commit_message>
Agrega grafica de asegurados por entidad
</commit_message>
<xml_diff>
--- a/data/asegurados_graph2.xlsx
+++ b/data/asegurados_graph2.xlsx
@@ -14,51 +14,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>entidad</t>
   </si>
   <si>
-    <t>dic-2024</t>
-  </si>
-  <si>
-    <t>may-2025</t>
-  </si>
-  <si>
-    <t>dif</t>
-  </si>
-  <si>
-    <t>dif_pct</t>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>tmac</t>
+  </si>
+  <si>
+    <t>participacion</t>
+  </si>
+  <si>
+    <t>CDMX</t>
+  </si>
+  <si>
+    <t>Jalisco</t>
+  </si>
+  <si>
+    <t>Nuevo León</t>
   </si>
   <si>
     <t>Estado México</t>
   </si>
   <si>
-    <t>Nuevo León</t>
-  </si>
-  <si>
-    <t>Jalisco</t>
+    <t>Guanajuato</t>
+  </si>
+  <si>
+    <t>Baja California</t>
+  </si>
+  <si>
+    <t>Chihuahua</t>
+  </si>
+  <si>
+    <t>Coahuila</t>
+  </si>
+  <si>
+    <t>Veracruz</t>
+  </si>
+  <si>
+    <t>Querétaro</t>
+  </si>
+  <si>
+    <t>Tamaulipas</t>
+  </si>
+  <si>
+    <t>Puebla</t>
+  </si>
+  <si>
+    <t>Sonora</t>
+  </si>
+  <si>
+    <t>Sinaloa</t>
   </si>
   <si>
     <t>Quintana Roo</t>
   </si>
   <si>
-    <t>Baja California</t>
-  </si>
-  <si>
-    <t>Sinaloa</t>
-  </si>
-  <si>
-    <t>Veracruz de Ignacio de la Llave</t>
+    <t>Michoacán</t>
+  </si>
+  <si>
+    <t>San Luis Potosí</t>
+  </si>
+  <si>
+    <t>Yucatán</t>
+  </si>
+  <si>
+    <t>Aguascalientes</t>
+  </si>
+  <si>
+    <t>Hidalgo</t>
+  </si>
+  <si>
+    <t>Chiapas</t>
+  </si>
+  <si>
+    <t>Durango</t>
+  </si>
+  <si>
+    <t>Oaxaca</t>
+  </si>
+  <si>
+    <t>Baja California Sur</t>
+  </si>
+  <si>
+    <t>Morelos</t>
+  </si>
+  <si>
+    <t>Tabasco</t>
+  </si>
+  <si>
+    <t>Zacatecas</t>
+  </si>
+  <si>
+    <t>Nayarit</t>
+  </si>
+  <si>
+    <t>Guerrero</t>
+  </si>
+  <si>
+    <t>Colima</t>
   </si>
   <si>
     <t>Campeche</t>
   </si>
   <si>
-    <t>Oaxaca</t>
-  </si>
-  <si>
-    <t>Guerrero</t>
+    <t>Tlaxcala</t>
   </si>
 </sst>
 </file>
@@ -416,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,142 +507,142 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1876507</v>
+        <v>3410553</v>
       </c>
       <c r="D2">
-        <v>1913529</v>
+        <v>3481080</v>
       </c>
       <c r="E2">
-        <v>37022</v>
+        <v>0.2928299435954962</v>
       </c>
       <c r="F2">
-        <v>1.972920964323608</v>
+        <v>15.55995509395565</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1915193</v>
+        <v>1752923</v>
       </c>
       <c r="D3">
-        <v>1942067</v>
+        <v>2044807</v>
       </c>
       <c r="E3">
-        <v>26874</v>
+        <v>2.22465194492325</v>
       </c>
       <c r="F3">
-        <v>1.403200617379032</v>
+        <v>9.140009737152315</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>2026081</v>
+        <v>1597150</v>
       </c>
       <c r="D4">
-        <v>2044807</v>
+        <v>1942067</v>
       </c>
       <c r="E4">
-        <v>18726</v>
+        <v>2.832694270674763</v>
       </c>
       <c r="F4">
-        <v>0.9242473524010145</v>
+        <v>8.680775882614927</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>512165</v>
+        <v>1599580</v>
       </c>
       <c r="D5">
-        <v>526777</v>
+        <v>1913529</v>
       </c>
       <c r="E5">
-        <v>14612</v>
+        <v>2.593167935424812</v>
       </c>
       <c r="F5">
-        <v>2.852986830415979</v>
+        <v>8.553214896233889</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1008302</v>
+        <v>978760</v>
       </c>
       <c r="D6">
-        <v>1021585</v>
+        <v>1123211</v>
       </c>
       <c r="E6">
-        <v>13283</v>
+        <v>1.986041107462766</v>
       </c>
       <c r="F6">
-        <v>1.317363250296042</v>
+        <v>5.020600710422347</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>605219</v>
+        <v>865847</v>
       </c>
       <c r="D7">
-        <v>584140</v>
+        <v>1021585</v>
       </c>
       <c r="E7">
-        <v>-21079</v>
+        <v>2.39102893662746</v>
       </c>
       <c r="F7">
-        <v>-3.482871489493886</v>
+        <v>4.566346284675642</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
-        <v>777756</v>
+        <v>878741</v>
       </c>
       <c r="D8">
-        <v>770370</v>
+        <v>969756</v>
       </c>
       <c r="E8">
-        <v>-7386</v>
+        <v>1.417876310029009</v>
       </c>
       <c r="F8">
-        <v>-0.9496551617731011</v>
+        <v>4.334677689709531</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -587,56 +653,496 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>135625</v>
+        <v>776222</v>
       </c>
       <c r="D9">
-        <v>128276</v>
+        <v>865109</v>
       </c>
       <c r="E9">
-        <v>-7349</v>
+        <v>1.560869834242284</v>
       </c>
       <c r="F9">
-        <v>-5.418617511520737</v>
+        <v>3.866919804019695</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10">
-        <v>236905</v>
+        <v>741109</v>
       </c>
       <c r="D10">
-        <v>231425</v>
+        <v>770370</v>
       </c>
       <c r="E10">
-        <v>-5480</v>
+        <v>0.5547215698066488</v>
       </c>
       <c r="F10">
-        <v>-2.313163504358287</v>
+        <v>3.443449333462781</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>163156</v>
+        <v>569699</v>
       </c>
       <c r="D11">
+        <v>714977</v>
+      </c>
+      <c r="E11">
+        <v>3.298109512295722</v>
+      </c>
+      <c r="F11">
+        <v>3.1958501422579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>663209</v>
+      </c>
+      <c r="D12">
+        <v>694136</v>
+      </c>
+      <c r="E12">
+        <v>0.6532347955432227</v>
+      </c>
+      <c r="F12">
+        <v>3.102693701120917</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>612217</v>
+      </c>
+      <c r="D13">
+        <v>660903</v>
+      </c>
+      <c r="E13">
+        <v>1.099143638006406</v>
+      </c>
+      <c r="F13">
+        <v>2.954146702017929</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>615130</v>
+      </c>
+      <c r="D14">
+        <v>656096</v>
+      </c>
+      <c r="E14">
+        <v>0.925304604537236</v>
+      </c>
+      <c r="F14">
+        <v>2.932660064498353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>536571</v>
+      </c>
+      <c r="D15">
+        <v>584140</v>
+      </c>
+      <c r="E15">
+        <v>1.220846332741865</v>
+      </c>
+      <c r="F15">
+        <v>2.611026511480131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>447177</v>
+      </c>
+      <c r="D16">
+        <v>526777</v>
+      </c>
+      <c r="E16">
+        <v>2.367926517916974</v>
+      </c>
+      <c r="F16">
+        <v>2.354621687674135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>438758</v>
+      </c>
+      <c r="D17">
+        <v>493018</v>
+      </c>
+      <c r="E17">
+        <v>1.679630902974871</v>
+      </c>
+      <c r="F17">
+        <v>2.203723539968006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>438994</v>
+      </c>
+      <c r="D18">
+        <v>482016</v>
+      </c>
+      <c r="E18">
+        <v>1.344552650428654</v>
+      </c>
+      <c r="F18">
+        <v>2.154546093329693</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>363698</v>
+      </c>
+      <c r="D19">
+        <v>437956</v>
+      </c>
+      <c r="E19">
+        <v>2.689746344488464</v>
+      </c>
+      <c r="F19">
+        <v>1.957603873834684</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>316019</v>
+      </c>
+      <c r="D20">
+        <v>366400</v>
+      </c>
+      <c r="E20">
+        <v>2.13567588984469</v>
+      </c>
+      <c r="F20">
+        <v>1.637758266522272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>227968</v>
+      </c>
+      <c r="D21">
+        <v>289428</v>
+      </c>
+      <c r="E21">
+        <v>3.46882615117392</v>
+      </c>
+      <c r="F21">
+        <v>1.293703874353188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>223360</v>
+      </c>
+      <c r="D22">
+        <v>261965</v>
+      </c>
+      <c r="E22">
+        <v>2.303648940799063</v>
+      </c>
+      <c r="F22">
+        <v>1.170947992056515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>248119</v>
+      </c>
+      <c r="D23">
+        <v>258828</v>
+      </c>
+      <c r="E23">
+        <v>0.6054724568105074</v>
+      </c>
+      <c r="F23">
+        <v>1.156926027858697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>212830</v>
+      </c>
+      <c r="D24">
+        <v>231425</v>
+      </c>
+      <c r="E24">
+        <v>1.203789662850263</v>
+      </c>
+      <c r="F24">
+        <v>1.034438337417895</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>180012</v>
+      </c>
+      <c r="D25">
+        <v>224416</v>
+      </c>
+      <c r="E25">
+        <v>3.199812583134221</v>
+      </c>
+      <c r="F25">
+        <v>1.003109058787834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>208261</v>
+      </c>
+      <c r="D26">
+        <v>220151</v>
+      </c>
+      <c r="E26">
+        <v>0.7963192288339638</v>
+      </c>
+      <c r="F26">
+        <v>0.9840450876996307</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>167249</v>
+      </c>
+      <c r="D27">
+        <v>203587</v>
+      </c>
+      <c r="E27">
+        <v>2.848526335453072</v>
+      </c>
+      <c r="F27">
+        <v>0.9100062560220246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>183796</v>
+      </c>
+      <c r="D28">
+        <v>189860</v>
+      </c>
+      <c r="E28">
+        <v>0.4647984461070065</v>
+      </c>
+      <c r="F28">
+        <v>0.8486484292628783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>140978</v>
+      </c>
+      <c r="D29">
+        <v>181889</v>
+      </c>
+      <c r="E29">
+        <v>3.706951930521174</v>
+      </c>
+      <c r="F29">
+        <v>0.8130191412103426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>160298</v>
+      </c>
+      <c r="D30">
         <v>159924</v>
       </c>
-      <c r="E11">
-        <v>-3232</v>
-      </c>
-      <c r="F11">
-        <v>-1.980926230111059</v>
+      <c r="E30">
+        <v>-0.03336415500921897</v>
+      </c>
+      <c r="F30">
+        <v>0.7148385726400324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>131595</v>
+      </c>
+      <c r="D31">
+        <v>156410</v>
+      </c>
+      <c r="E31">
+        <v>2.498586275645431</v>
+      </c>
+      <c r="F31">
+        <v>0.6991314696144885</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>122144</v>
+      </c>
+      <c r="D32">
+        <v>128276</v>
+      </c>
+      <c r="E32">
+        <v>0.7022185868674757</v>
+      </c>
+      <c r="F32">
+        <v>0.5733763083963183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>99105</v>
+      </c>
+      <c r="D33">
+        <v>117952</v>
+      </c>
+      <c r="E33">
+        <v>2.518299051230533</v>
+      </c>
+      <c r="F33">
+        <v>0.5272294297293533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>